<commit_message>
Experimentación, falta limpiar código
Co-Authored-By: Carlos Ponce <89041361+carlos-p11@users.noreply.github.com>
Co-Authored-By: JuanGtz030701 <70152183+JuanGtz030701@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Data/SP500 List/sp500.xlsx
+++ b/Data/SP500 List/sp500.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\ITESO\7mo Semestre\PAP de Modelación Matemática\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/if728143_iteso_mx/Documents/ITESO/8 Semestre/PAP 2/valuation_model/Data/SP500 List/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405414B1-6FCB-4016-9962-0610A57D9727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{405414B1-6FCB-4016-9962-0610A57D9727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F8FBABC-7940-9D4F-B8AB-1AA54C335408}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sp500" sheetId="1" r:id="rId1"/>
@@ -4264,15 +4264,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:XFD200"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4300,7 +4301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4314,7 +4315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4328,7 +4329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -4356,7 +4357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4370,7 +4371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -4398,7 +4399,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -4426,7 +4427,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -4440,7 +4441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -4454,7 +4455,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -4468,7 +4469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -4496,7 +4497,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4510,7 +4511,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -4524,7 +4525,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -4538,7 +4539,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4566,7 +4567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -4580,7 +4581,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -4594,7 +4595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -4608,7 +4609,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -4636,7 +4637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -4678,7 +4679,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -4692,7 +4693,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -4706,7 +4707,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -4720,7 +4721,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -4748,7 +4749,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -4762,7 +4763,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -4790,7 +4791,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -4804,7 +4805,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -4818,7 +4819,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -4860,7 +4861,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -4874,7 +4875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>129</v>
       </c>
@@ -4888,7 +4889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -4916,7 +4917,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -4930,7 +4931,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -4944,7 +4945,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -4958,7 +4959,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -4972,7 +4973,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>151</v>
       </c>
@@ -4986,7 +4987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>153</v>
       </c>
@@ -5000,7 +5001,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -5028,7 +5029,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -5042,7 +5043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>164</v>
       </c>
@@ -5056,7 +5057,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>167</v>
       </c>
@@ -5070,7 +5071,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>170</v>
       </c>
@@ -5084,7 +5085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>172</v>
       </c>
@@ -5098,7 +5099,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>175</v>
       </c>
@@ -5112,7 +5113,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>178</v>
       </c>
@@ -5126,7 +5127,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>181</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>183</v>
       </c>
@@ -5154,7 +5155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>185</v>
       </c>
@@ -5168,7 +5169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>187</v>
       </c>
@@ -5182,7 +5183,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>189</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>192</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>195</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>198</v>
       </c>
@@ -5238,7 +5239,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>200</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>202</v>
       </c>
@@ -5266,7 +5267,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>204</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>206</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>209</v>
       </c>
@@ -5308,7 +5309,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>211</v>
       </c>
@@ -5322,7 +5323,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>213</v>
       </c>
@@ -5336,7 +5337,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>215</v>
       </c>
@@ -5350,7 +5351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>217</v>
       </c>
@@ -5364,7 +5365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>219</v>
       </c>
@@ -5378,7 +5379,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>221</v>
       </c>
@@ -5392,7 +5393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>223</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>225</v>
       </c>
@@ -5420,7 +5421,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>228</v>
       </c>
@@ -5434,7 +5435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>230</v>
       </c>
@@ -5448,7 +5449,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>233</v>
       </c>
@@ -5462,7 +5463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>235</v>
       </c>
@@ -5476,7 +5477,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>238</v>
       </c>
@@ -5490,7 +5491,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>240</v>
       </c>
@@ -5504,7 +5505,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>243</v>
       </c>
@@ -5518,7 +5519,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>245</v>
       </c>
@@ -5532,7 +5533,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>247</v>
       </c>
@@ -5546,7 +5547,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>249</v>
       </c>
@@ -5560,7 +5561,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>252</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>254</v>
       </c>
@@ -5588,7 +5589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>256</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>259</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>262</v>
       </c>
@@ -5630,7 +5631,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>265</v>
       </c>
@@ -5644,7 +5645,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>267</v>
       </c>
@@ -5658,7 +5659,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>269</v>
       </c>
@@ -5672,7 +5673,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>272</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>274</v>
       </c>
@@ -5700,7 +5701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>276</v>
       </c>
@@ -5714,7 +5715,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>279</v>
       </c>
@@ -5728,7 +5729,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>281</v>
       </c>
@@ -5742,7 +5743,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>284</v>
       </c>
@@ -5756,7 +5757,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>287</v>
       </c>
@@ -5770,7 +5771,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>290</v>
       </c>
@@ -5784,7 +5785,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>293</v>
       </c>
@@ -5798,7 +5799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>295</v>
       </c>
@@ -5812,7 +5813,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>298</v>
       </c>
@@ -5826,7 +5827,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>300</v>
       </c>
@@ -5840,7 +5841,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>302</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>305</v>
       </c>
@@ -5868,7 +5869,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>307</v>
       </c>
@@ -5882,7 +5883,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>309</v>
       </c>
@@ -5896,7 +5897,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>312</v>
       </c>
@@ -5910,7 +5911,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>314</v>
       </c>
@@ -5924,7 +5925,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>316</v>
       </c>
@@ -5938,7 +5939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>318</v>
       </c>
@@ -5952,7 +5953,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>321</v>
       </c>
@@ -5966,7 +5967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>323</v>
       </c>
@@ -5980,7 +5981,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>325</v>
       </c>
@@ -5994,7 +5995,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>327</v>
       </c>
@@ -6008,7 +6009,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>329</v>
       </c>
@@ -6022,7 +6023,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>331</v>
       </c>
@@ -6036,7 +6037,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>333</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>335</v>
       </c>
@@ -6064,7 +6065,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>337</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>339</v>
       </c>
@@ -6092,7 +6093,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>341</v>
       </c>
@@ -6106,7 +6107,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>343</v>
       </c>
@@ -6120,7 +6121,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>345</v>
       </c>
@@ -6134,7 +6135,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>347</v>
       </c>
@@ -6148,7 +6149,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>350</v>
       </c>
@@ -6162,7 +6163,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>353</v>
       </c>
@@ -6176,7 +6177,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>355</v>
       </c>
@@ -6190,7 +6191,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>357</v>
       </c>
@@ -6204,7 +6205,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>359</v>
       </c>
@@ -6218,7 +6219,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>362</v>
       </c>
@@ -6232,7 +6233,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>365</v>
       </c>
@@ -6246,7 +6247,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>368</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>370</v>
       </c>
@@ -6274,7 +6275,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>372</v>
       </c>
@@ -6288,7 +6289,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>375</v>
       </c>
@@ -6302,7 +6303,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>378</v>
       </c>
@@ -6316,7 +6317,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>380</v>
       </c>
@@ -6330,7 +6331,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>382</v>
       </c>
@@ -6344,7 +6345,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>384</v>
       </c>
@@ -6358,7 +6359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>386</v>
       </c>
@@ -6372,7 +6373,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>388</v>
       </c>
@@ -6386,7 +6387,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>390</v>
       </c>
@@ -6400,7 +6401,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>392</v>
       </c>
@@ -6414,7 +6415,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>394</v>
       </c>
@@ -6428,7 +6429,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>397</v>
       </c>
@@ -6442,7 +6443,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>400</v>
       </c>
@@ -6456,7 +6457,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>402</v>
       </c>
@@ -6470,7 +6471,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>404</v>
       </c>
@@ -6484,7 +6485,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>406</v>
       </c>
@@ -6498,7 +6499,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>408</v>
       </c>
@@ -6512,7 +6513,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>411</v>
       </c>
@@ -6526,7 +6527,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>413</v>
       </c>
@@ -6540,7 +6541,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>415</v>
       </c>
@@ -6554,7 +6555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>417</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>419</v>
       </c>
@@ -6582,7 +6583,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>422</v>
       </c>
@@ -6596,7 +6597,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>424</v>
       </c>
@@ -6610,7 +6611,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>426</v>
       </c>
@@ -6624,7 +6625,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>428</v>
       </c>
@@ -6638,7 +6639,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>430</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>432</v>
       </c>
@@ -6666,7 +6667,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>434</v>
       </c>
@@ -6680,7 +6681,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>436</v>
       </c>
@@ -6694,7 +6695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>438</v>
       </c>
@@ -6708,7 +6709,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>440</v>
       </c>
@@ -6722,7 +6723,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>442</v>
       </c>
@@ -6736,7 +6737,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>444</v>
       </c>
@@ -6750,7 +6751,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>446</v>
       </c>
@@ -6764,7 +6765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>448</v>
       </c>
@@ -6778,7 +6779,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>449</v>
       </c>
@@ -6792,7 +6793,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>451</v>
       </c>
@@ -6806,7 +6807,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>453</v>
       </c>
@@ -6820,7 +6821,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>455</v>
       </c>
@@ -6834,7 +6835,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>457</v>
       </c>
@@ -6848,7 +6849,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>460</v>
       </c>
@@ -6862,7 +6863,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1129</v>
       </c>
@@ -6876,7 +6877,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>462</v>
       </c>
@@ -6890,7 +6891,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>464</v>
       </c>
@@ -6904,7 +6905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>466</v>
       </c>
@@ -6918,7 +6919,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>468</v>
       </c>
@@ -6932,7 +6933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>470</v>
       </c>
@@ -6946,7 +6947,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>472</v>
       </c>
@@ -6960,7 +6961,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>474</v>
       </c>
@@ -6974,7 +6975,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>476</v>
       </c>
@@ -6988,7 +6989,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>478</v>
       </c>
@@ -7002,7 +7003,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>480</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>482</v>
       </c>
@@ -7030,7 +7031,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>485</v>
       </c>
@@ -7044,7 +7045,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>487</v>
       </c>
@@ -7058,7 +7059,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>489</v>
       </c>
@@ -7072,7 +7073,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>491</v>
       </c>
@@ -7086,7 +7087,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>1131</v>
       </c>
@@ -7100,7 +7101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>493</v>
       </c>
@@ -7114,7 +7115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>495</v>
       </c>
@@ -7128,7 +7129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>497</v>
       </c>
@@ -7142,7 +7143,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>499</v>
       </c>
@@ -7156,7 +7157,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>502</v>
       </c>
@@ -7170,7 +7171,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>505</v>
       </c>
@@ -7184,7 +7185,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>507</v>
       </c>
@@ -7198,7 +7199,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>509</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>511</v>
       </c>
@@ -7226,7 +7227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>513</v>
       </c>
@@ -7240,7 +7241,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>516</v>
       </c>
@@ -7254,7 +7255,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>519</v>
       </c>
@@ -7268,7 +7269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>521</v>
       </c>
@@ -7282,7 +7283,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>524</v>
       </c>
@@ -7296,7 +7297,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>526</v>
       </c>
@@ -7310,7 +7311,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>528</v>
       </c>
@@ -7324,7 +7325,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>530</v>
       </c>
@@ -7338,7 +7339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>532</v>
       </c>
@@ -7352,7 +7353,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>534</v>
       </c>
@@ -7366,7 +7367,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -7380,7 +7381,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>538</v>
       </c>
@@ -7394,7 +7395,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>540</v>
       </c>
@@ -7408,7 +7409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>542</v>
       </c>
@@ -7422,7 +7423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>544</v>
       </c>
@@ -7436,7 +7437,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>546</v>
       </c>
@@ -7450,7 +7451,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>548</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>550</v>
       </c>
@@ -7478,7 +7479,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>553</v>
       </c>
@@ -7492,7 +7493,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>555</v>
       </c>
@@ -7506,7 +7507,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>558</v>
       </c>
@@ -7520,7 +7521,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>560</v>
       </c>
@@ -7534,7 +7535,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>562</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>564</v>
       </c>
@@ -7562,7 +7563,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>566</v>
       </c>
@@ -7576,7 +7577,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>568</v>
       </c>
@@ -7590,7 +7591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>570</v>
       </c>
@@ -7604,7 +7605,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>573</v>
       </c>
@@ -7618,7 +7619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>575</v>
       </c>
@@ -7632,7 +7633,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>577</v>
       </c>
@@ -7646,7 +7647,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>580</v>
       </c>
@@ -7660,7 +7661,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>582</v>
       </c>
@@ -7674,7 +7675,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>584</v>
       </c>
@@ -7688,7 +7689,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>586</v>
       </c>
@@ -7702,7 +7703,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>588</v>
       </c>
@@ -7716,7 +7717,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>590</v>
       </c>
@@ -7730,7 +7731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>591</v>
       </c>
@@ -7744,7 +7745,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>593</v>
       </c>
@@ -7758,7 +7759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>595</v>
       </c>
@@ -7772,7 +7773,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>597</v>
       </c>
@@ -7786,7 +7787,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>599</v>
       </c>
@@ -7800,7 +7801,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>601</v>
       </c>
@@ -7814,7 +7815,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>603</v>
       </c>
@@ -7828,7 +7829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>605</v>
       </c>
@@ -7842,7 +7843,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>607</v>
       </c>
@@ -7856,7 +7857,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>609</v>
       </c>
@@ -7870,7 +7871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>611</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>613</v>
       </c>
@@ -7898,7 +7899,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>616</v>
       </c>
@@ -7912,7 +7913,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>618</v>
       </c>
@@ -7926,7 +7927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>620</v>
       </c>
@@ -7940,7 +7941,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>622</v>
       </c>
@@ -7954,7 +7955,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>624</v>
       </c>
@@ -7968,7 +7969,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>626</v>
       </c>
@@ -7982,7 +7983,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>628</v>
       </c>
@@ -7996,7 +7997,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>631</v>
       </c>
@@ -8010,7 +8011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>633</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>636</v>
       </c>
@@ -8038,7 +8039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>638</v>
       </c>
@@ -8052,7 +8053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>640</v>
       </c>
@@ -8066,7 +8067,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>642</v>
       </c>
@@ -8080,7 +8081,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>644</v>
       </c>
@@ -8094,7 +8095,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>646</v>
       </c>
@@ -8108,7 +8109,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>648</v>
       </c>
@@ -8122,7 +8123,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>650</v>
       </c>
@@ -8136,7 +8137,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>653</v>
       </c>
@@ -8150,7 +8151,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>655</v>
       </c>
@@ -8164,7 +8165,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>657</v>
       </c>
@@ -8178,7 +8179,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>660</v>
       </c>
@@ -8192,7 +8193,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>662</v>
       </c>
@@ -8206,7 +8207,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>664</v>
       </c>
@@ -8220,7 +8221,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>667</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>669</v>
       </c>
@@ -8248,7 +8249,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>671</v>
       </c>
@@ -8262,7 +8263,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>673</v>
       </c>
@@ -8276,7 +8277,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>675</v>
       </c>
@@ -8290,7 +8291,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>677</v>
       </c>
@@ -8304,7 +8305,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>679</v>
       </c>
@@ -8318,7 +8319,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>681</v>
       </c>
@@ -8332,7 +8333,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>683</v>
       </c>
@@ -8346,7 +8347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>685</v>
       </c>
@@ -8360,7 +8361,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>687</v>
       </c>
@@ -8374,7 +8375,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>690</v>
       </c>
@@ -8388,7 +8389,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>692</v>
       </c>
@@ -8402,7 +8403,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>694</v>
       </c>
@@ -8416,7 +8417,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>696</v>
       </c>
@@ -8430,7 +8431,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>699</v>
       </c>
@@ -8444,7 +8445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>701</v>
       </c>
@@ -8458,7 +8459,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>703</v>
       </c>
@@ -8472,7 +8473,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>705</v>
       </c>
@@ -8486,7 +8487,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>708</v>
       </c>
@@ -8500,7 +8501,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>710</v>
       </c>
@@ -8514,7 +8515,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>712</v>
       </c>
@@ -8528,7 +8529,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>714</v>
       </c>
@@ -8542,7 +8543,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>717</v>
       </c>
@@ -8556,7 +8557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>719</v>
       </c>
@@ -8570,7 +8571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>721</v>
       </c>
@@ -8584,7 +8585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>723</v>
       </c>
@@ -8598,7 +8599,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>725</v>
       </c>
@@ -8612,7 +8613,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>727</v>
       </c>
@@ -8626,7 +8627,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>729</v>
       </c>
@@ -8640,7 +8641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>731</v>
       </c>
@@ -8654,7 +8655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>733</v>
       </c>
@@ -8668,7 +8669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>735</v>
       </c>
@@ -8682,7 +8683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>737</v>
       </c>
@@ -8696,7 +8697,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>739</v>
       </c>
@@ -8710,7 +8711,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>741</v>
       </c>
@@ -8724,7 +8725,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>743</v>
       </c>
@@ -8738,7 +8739,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>745</v>
       </c>
@@ -8752,7 +8753,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>747</v>
       </c>
@@ -8766,7 +8767,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>749</v>
       </c>
@@ -8780,7 +8781,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>751</v>
       </c>
@@ -8794,7 +8795,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>754</v>
       </c>
@@ -8808,7 +8809,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>756</v>
       </c>
@@ -8822,7 +8823,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>759</v>
       </c>
@@ -8836,7 +8837,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>761</v>
       </c>
@@ -8850,7 +8851,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>763</v>
       </c>
@@ -8864,7 +8865,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>765</v>
       </c>
@@ -8878,7 +8879,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>767</v>
       </c>
@@ -8892,7 +8893,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>769</v>
       </c>
@@ -8906,7 +8907,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>771</v>
       </c>
@@ -8920,7 +8921,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>773</v>
       </c>
@@ -8934,7 +8935,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>774</v>
       </c>
@@ -8948,7 +8949,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>776</v>
       </c>
@@ -8962,7 +8963,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>778</v>
       </c>
@@ -8976,7 +8977,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>780</v>
       </c>
@@ -8990,7 +8991,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>783</v>
       </c>
@@ -9004,7 +9005,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>786</v>
       </c>
@@ -9018,7 +9019,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>789</v>
       </c>
@@ -9032,7 +9033,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>791</v>
       </c>
@@ -9046,7 +9047,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>793</v>
       </c>
@@ -9060,7 +9061,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>796</v>
       </c>
@@ -9074,7 +9075,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>798</v>
       </c>
@@ -9088,7 +9089,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>800</v>
       </c>
@@ -9102,7 +9103,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>802</v>
       </c>
@@ -9116,7 +9117,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>804</v>
       </c>
@@ -9130,7 +9131,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>806</v>
       </c>
@@ -9144,7 +9145,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>808</v>
       </c>
@@ -9158,7 +9159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>810</v>
       </c>
@@ -9172,7 +9173,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>813</v>
       </c>
@@ -9186,7 +9187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>815</v>
       </c>
@@ -9200,7 +9201,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>817</v>
       </c>
@@ -9214,7 +9215,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>819</v>
       </c>
@@ -9228,7 +9229,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>821</v>
       </c>
@@ -9242,7 +9243,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>823</v>
       </c>
@@ -9256,7 +9257,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>825</v>
       </c>
@@ -9270,7 +9271,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>827</v>
       </c>
@@ -9284,7 +9285,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>829</v>
       </c>
@@ -9298,7 +9299,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>831</v>
       </c>
@@ -9312,7 +9313,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>833</v>
       </c>
@@ -9326,7 +9327,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>835</v>
       </c>
@@ -9340,7 +9341,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>837</v>
       </c>
@@ -9354,7 +9355,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>839</v>
       </c>
@@ -9368,7 +9369,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>841</v>
       </c>
@@ -9382,7 +9383,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>843</v>
       </c>
@@ -9396,7 +9397,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>845</v>
       </c>
@@ -9410,7 +9411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>847</v>
       </c>
@@ -9424,7 +9425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>849</v>
       </c>
@@ -9438,7 +9439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>851</v>
       </c>
@@ -9452,7 +9453,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>853</v>
       </c>
@@ -9466,7 +9467,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>1127</v>
       </c>
@@ -9480,7 +9481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>855</v>
       </c>
@@ -9494,7 +9495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>857</v>
       </c>
@@ -9508,7 +9509,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>859</v>
       </c>
@@ -9522,7 +9523,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>861</v>
       </c>
@@ -9536,7 +9537,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>863</v>
       </c>
@@ -9550,7 +9551,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>865</v>
       </c>
@@ -9564,7 +9565,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>867</v>
       </c>
@@ -9578,7 +9579,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>869</v>
       </c>
@@ -9592,7 +9593,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>871</v>
       </c>
@@ -9606,7 +9607,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>873</v>
       </c>
@@ -9620,7 +9621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>875</v>
       </c>
@@ -9634,7 +9635,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>877</v>
       </c>
@@ -9648,7 +9649,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>879</v>
       </c>
@@ -9662,7 +9663,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>881</v>
       </c>
@@ -9676,7 +9677,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>884</v>
       </c>
@@ -9690,7 +9691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>886</v>
       </c>
@@ -9704,7 +9705,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>888</v>
       </c>
@@ -9718,7 +9719,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>889</v>
       </c>
@@ -9732,7 +9733,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>891</v>
       </c>
@@ -9746,7 +9747,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>893</v>
       </c>
@@ -9760,7 +9761,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>895</v>
       </c>
@@ -9774,7 +9775,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>897</v>
       </c>
@@ -9788,7 +9789,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>899</v>
       </c>
@@ -9802,7 +9803,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>901</v>
       </c>
@@ -9816,7 +9817,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>903</v>
       </c>
@@ -9830,7 +9831,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>905</v>
       </c>
@@ -9844,7 +9845,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>907</v>
       </c>
@@ -9858,7 +9859,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>909</v>
       </c>
@@ -9872,7 +9873,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>911</v>
       </c>
@@ -9886,7 +9887,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>913</v>
       </c>
@@ -9900,7 +9901,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>915</v>
       </c>
@@ -9914,7 +9915,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>918</v>
       </c>
@@ -9928,7 +9929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>920</v>
       </c>
@@ -9942,7 +9943,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>923</v>
       </c>
@@ -9956,7 +9957,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>925</v>
       </c>
@@ -9970,7 +9971,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>927</v>
       </c>
@@ -9984,7 +9985,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>929</v>
       </c>
@@ -9998,7 +9999,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>932</v>
       </c>
@@ -10012,7 +10013,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>934</v>
       </c>
@@ -10026,7 +10027,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>936</v>
       </c>
@@ -10040,7 +10041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>938</v>
       </c>
@@ -10054,7 +10055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>940</v>
       </c>
@@ -10068,7 +10069,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>942</v>
       </c>
@@ -10082,7 +10083,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>944</v>
       </c>
@@ -10096,7 +10097,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>946</v>
       </c>
@@ -10110,7 +10111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>948</v>
       </c>
@@ -10124,7 +10125,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>950</v>
       </c>
@@ -10138,7 +10139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>952</v>
       </c>
@@ -10152,7 +10153,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>954</v>
       </c>
@@ -10166,7 +10167,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>956</v>
       </c>
@@ -10180,7 +10181,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>958</v>
       </c>
@@ -10194,7 +10195,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>960</v>
       </c>
@@ -10208,7 +10209,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>962</v>
       </c>
@@ -10222,7 +10223,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>964</v>
       </c>
@@ -10236,7 +10237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>966</v>
       </c>
@@ -10250,7 +10251,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>968</v>
       </c>
@@ -10264,7 +10265,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>970</v>
       </c>
@@ -10278,7 +10279,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>972</v>
       </c>
@@ -10292,7 +10293,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>974</v>
       </c>
@@ -10306,7 +10307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>976</v>
       </c>
@@ -10320,7 +10321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>978</v>
       </c>
@@ -10334,7 +10335,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>980</v>
       </c>
@@ -10348,7 +10349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>982</v>
       </c>
@@ -10362,7 +10363,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>985</v>
       </c>
@@ -10376,7 +10377,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>988</v>
       </c>
@@ -10390,7 +10391,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>990</v>
       </c>
@@ -10404,7 +10405,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>992</v>
       </c>
@@ -10418,7 +10419,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>994</v>
       </c>
@@ -10432,7 +10433,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>996</v>
       </c>
@@ -10446,7 +10447,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>998</v>
       </c>
@@ -10460,7 +10461,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>1001</v>
       </c>
@@ -10474,7 +10475,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>1003</v>
       </c>
@@ -10488,7 +10489,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>1005</v>
       </c>
@@ -10502,7 +10503,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>1007</v>
       </c>
@@ -10516,7 +10517,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>1009</v>
       </c>
@@ -10530,7 +10531,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>1011</v>
       </c>
@@ -10544,7 +10545,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>1013</v>
       </c>
@@ -10558,7 +10559,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>1015</v>
       </c>
@@ -10572,7 +10573,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>1017</v>
       </c>
@@ -10586,7 +10587,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>1019</v>
       </c>
@@ -10600,7 +10601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>1021</v>
       </c>
@@ -10614,7 +10615,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>1023</v>
       </c>
@@ -10628,7 +10629,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>1025</v>
       </c>
@@ -10642,7 +10643,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>1027</v>
       </c>
@@ -10656,7 +10657,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>1029</v>
       </c>
@@ -10670,7 +10671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>1031</v>
       </c>
@@ -10684,7 +10685,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>1033</v>
       </c>
@@ -10698,7 +10699,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>1035</v>
       </c>
@@ -10712,7 +10713,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>1037</v>
       </c>
@@ -10726,7 +10727,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>1039</v>
       </c>
@@ -10740,7 +10741,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>1041</v>
       </c>
@@ -10754,7 +10755,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>1043</v>
       </c>
@@ -10768,7 +10769,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>1045</v>
       </c>
@@ -10782,7 +10783,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>1048</v>
       </c>
@@ -10796,7 +10797,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>1050</v>
       </c>
@@ -10810,7 +10811,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>1052</v>
       </c>
@@ -10824,7 +10825,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>1054</v>
       </c>
@@ -10838,7 +10839,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>1056</v>
       </c>
@@ -10852,7 +10853,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>1058</v>
       </c>
@@ -10866,7 +10867,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>1060</v>
       </c>
@@ -10880,7 +10881,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>1062</v>
       </c>
@@ -10894,7 +10895,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="474" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>1064</v>
       </c>
@@ -10908,7 +10909,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>1066</v>
       </c>
@@ -10922,7 +10923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>1068</v>
       </c>
@@ -10936,7 +10937,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>1070</v>
       </c>
@@ -10950,7 +10951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>1072</v>
       </c>
@@ -10964,7 +10965,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>1074</v>
       </c>
@@ -10978,7 +10979,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="480" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>1076</v>
       </c>
@@ -10992,7 +10993,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>1079</v>
       </c>
@@ -11006,7 +11007,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>1081</v>
       </c>
@@ -11020,7 +11021,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>1084</v>
       </c>
@@ -11034,7 +11035,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>1086</v>
       </c>
@@ -11048,7 +11049,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>1088</v>
       </c>
@@ -11062,7 +11063,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>1090</v>
       </c>
@@ -11076,7 +11077,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>1092</v>
       </c>
@@ -11090,7 +11091,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>1094</v>
       </c>
@@ -11104,7 +11105,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>1096</v>
       </c>
@@ -11118,7 +11119,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>1098</v>
       </c>
@@ -11132,7 +11133,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>1100</v>
       </c>
@@ -11146,7 +11147,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>1102</v>
       </c>
@@ -11160,7 +11161,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>1105</v>
       </c>
@@ -11174,7 +11175,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>1107</v>
       </c>
@@ -11188,7 +11189,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="495" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>1109</v>
       </c>
@@ -11202,7 +11203,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="496" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>1111</v>
       </c>
@@ -11216,7 +11217,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="497" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>1113</v>
       </c>
@@ -11230,7 +11231,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="498" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>1115</v>
       </c>
@@ -11244,7 +11245,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="499" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>1117</v>
       </c>
@@ -11258,7 +11259,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="500" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>1119</v>
       </c>
@@ -11272,7 +11273,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="501" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>1121</v>
       </c>
@@ -11286,7 +11287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="502" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>1123</v>
       </c>
@@ -11300,7 +11301,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="503" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>1125</v>
       </c>
@@ -11315,7 +11316,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D503" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D503" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="XRAY"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>